<commit_message>
Added Order Type test (eventough we have yet to decide the timestamp in order for the test to work propertly) and bugs in prevoous test fixed
</commit_message>
<xml_diff>
--- a/docs/GE3_TestCasesTemplate_2023_v1.0.xlsx
+++ b/docs/GE3_TestCasesTemplate_2023_v1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edu/PycharmProjects/G89.2023.T20.EG3/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\OneDrive\Escritorio\Desarrollo de Software\G89.2023.T20.EG3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5C936D-26EC-4A44-9994-B07B47458C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922B4995-BA05-45C2-A004-3B4754C13E53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="1515" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GE3 2023 F1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="125">
   <si>
     <t>#</t>
   </si>
@@ -92,9 +92,6 @@
     <t>"C/LISBOA,4, MADRID, SPAIN"</t>
   </si>
   <si>
-    <t>"+34123456789"</t>
-  </si>
-  <si>
     <t>"28005"</t>
   </si>
   <si>
@@ -107,40 +104,16 @@
     <t>CE_NV_2</t>
   </si>
   <si>
-    <t>PRODUCT ID NOT NUMBER</t>
-  </si>
-  <si>
     <t>842169142322A</t>
   </si>
   <si>
     <t>"PREMIUM"</t>
   </si>
   <si>
-    <t>Exception: Product Id not valid</t>
-  </si>
-  <si>
     <t>CE_NV_3</t>
   </si>
   <si>
     <t>PRODUCT ID NOT CHECK SUM</t>
-  </si>
-  <si>
-    <t>CE_V_8</t>
-  </si>
-  <si>
-    <t>ecc7f631f98930aca6e183c6e505dFFF</t>
-  </si>
-  <si>
-    <t>CE_NV_9</t>
-  </si>
-  <si>
-    <t>ORDER_TYPE WRONG</t>
-  </si>
-  <si>
-    <t>"PRE"</t>
-  </si>
-  <si>
-    <t>Exception : order type wrong</t>
   </si>
   <si>
     <t>OUTPUT</t>
@@ -211,28 +184,229 @@
     <t>Path considering that the input is not found in the file</t>
   </si>
   <si>
-    <t>PRODUCT ID EMPTY</t>
-  </si>
-  <si>
-    <t>NULL</t>
-  </si>
-  <si>
-    <t>CE_NV_4</t>
-  </si>
-  <si>
-    <t>too long</t>
-  </si>
-  <si>
-    <t>too short</t>
-  </si>
-  <si>
-    <t>limites x2</t>
-  </si>
-  <si>
-    <t>falta alto</t>
-  </si>
-  <si>
-    <t>todo bien</t>
+    <t>"regular"</t>
+  </si>
+  <si>
+    <t>"premiums"</t>
+  </si>
+  <si>
+    <t>PRODUCT ID NOT (EA13)NUMBER</t>
+  </si>
+  <si>
+    <t>"regula"</t>
+  </si>
+  <si>
+    <t>ORDER_TYPE NOT VALID (not a string)</t>
+  </si>
+  <si>
+    <t>ADDRES</t>
+  </si>
+  <si>
+    <t>CE_V_12</t>
+  </si>
+  <si>
+    <t>CE_NV_13</t>
+  </si>
+  <si>
+    <t>ADDRESS_NO_SPACES</t>
+  </si>
+  <si>
+    <t>"C/LISBOA4MADRIDSPAIN"</t>
+  </si>
+  <si>
+    <t>Exception: Addres must contain a space</t>
+  </si>
+  <si>
+    <t>CE_NV_14</t>
+  </si>
+  <si>
+    <t>ADDRES_TYPE WRONG</t>
+  </si>
+  <si>
+    <t>Exception: Address type must by str</t>
+  </si>
+  <si>
+    <t>CE_NV_15</t>
+  </si>
+  <si>
+    <t>ADDRES_LENGTH SMALL</t>
+  </si>
+  <si>
+    <t>"MICASA, MADRID"</t>
+  </si>
+  <si>
+    <t>Exception: Address too short</t>
+  </si>
+  <si>
+    <t>CE_NV_16</t>
+  </si>
+  <si>
+    <t>ADDRES_LENGTH BIG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"CALLE DE NUESTRO SEÑOR SATORU GOJO EL BENEVOLENTE QUE CON SUS ARTES MARCIALES Y SU ESPECIAL AURA MURIÓ, MADRID, ESPAÑA"  </t>
+  </si>
+  <si>
+    <t>Exception: Address too long</t>
+  </si>
+  <si>
+    <t>CE_NV_8</t>
+  </si>
+  <si>
+    <t>CE_NV_9</t>
+  </si>
+  <si>
+    <t>CE_NV_10</t>
+  </si>
+  <si>
+    <t>CE_V_5</t>
+  </si>
+  <si>
+    <t>CE_V_6</t>
+  </si>
+  <si>
+    <t>PHONE_NUMBER_TYPE NOT VALID</t>
+  </si>
+  <si>
+    <t>ORDER_TYPE NOT VALID TOO LONG</t>
+  </si>
+  <si>
+    <t>ORDER_TYPE NOT VALID TOO SHORT</t>
+  </si>
+  <si>
+    <t>CE_V_17</t>
+  </si>
+  <si>
+    <t>"DEATH_STAR"</t>
+  </si>
+  <si>
+    <t>Exception: Phone_number is not a number</t>
+  </si>
+  <si>
+    <t>"123456789"</t>
+  </si>
+  <si>
+    <t>CE_NV_18</t>
+  </si>
+  <si>
+    <t>VALD</t>
+  </si>
+  <si>
+    <t>CE_V_19</t>
+  </si>
+  <si>
+    <t>PHONE_NUMBER VALID</t>
+  </si>
+  <si>
+    <t>¿Valid Phone number?</t>
+  </si>
+  <si>
+    <t>CE_NV_XX</t>
+  </si>
+  <si>
+    <t>PHONE_NUMBER TOO SHORT</t>
+  </si>
+  <si>
+    <t>"123456"</t>
+  </si>
+  <si>
+    <t>Exception: Phone_number too short</t>
+  </si>
+  <si>
+    <t>PHONE_NUMBER TOO LONG</t>
+  </si>
+  <si>
+    <t>"123456789123456"</t>
+  </si>
+  <si>
+    <t>Exception: Phone_number too long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOT VALID </t>
+  </si>
+  <si>
+    <t>ZIP_CODE BELLOW 01000</t>
+  </si>
+  <si>
+    <t>Exception: Zip_Code bellow smallest valid (01000)</t>
+  </si>
+  <si>
+    <t>ZIP_CODE ABOVE 52999</t>
+  </si>
+  <si>
+    <t>Exception: Zip_Code above biggest valid (52999)</t>
+  </si>
+  <si>
+    <t>ZIP_CODE TOO FEW DIGITS</t>
+  </si>
+  <si>
+    <t>Exception: Zip_Code too few digits</t>
+  </si>
+  <si>
+    <t>ZIP_CODE NON INTEGER VALUE</t>
+  </si>
+  <si>
+    <t>Exception: Zip_Code must be an integer {01000-52999}</t>
+  </si>
+  <si>
+    <t>"942"</t>
+  </si>
+  <si>
+    <t>"53942"</t>
+  </si>
+  <si>
+    <t>"2382"</t>
+  </si>
+  <si>
+    <t>"La casa de paco"</t>
+  </si>
+  <si>
+    <t>ZIP_CODE FLOAT VALUE</t>
+  </si>
+  <si>
+    <t>"23.82"</t>
+  </si>
+  <si>
+    <t>Exception: Phone_number is not of type FLOAT</t>
+  </si>
+  <si>
+    <t>"123456.789123456"</t>
+  </si>
+  <si>
+    <t>Exception: Order Type Value too long</t>
+  </si>
+  <si>
+    <t>Exception: Order Type value is not a string</t>
+  </si>
+  <si>
+    <t>Exception: Order Type Value too short</t>
+  </si>
+  <si>
+    <t>"654314159"</t>
+  </si>
+  <si>
+    <t>PRODUCT ID TOO SHORT</t>
+  </si>
+  <si>
+    <t>PRODUCT ID TOO LONG</t>
+  </si>
+  <si>
+    <t>Exception: Product Id not valid, not an EAN13 code</t>
+  </si>
+  <si>
+    <t>Exception: Product Id not valid, id too short</t>
+  </si>
+  <si>
+    <t>Exception: Product Id not valid, id too long</t>
+  </si>
+  <si>
+    <t>Exception: Product Id not valid, id must be numeric</t>
+  </si>
+  <si>
+    <t>e01521684a7f9535e9fa098a2b86565f</t>
+  </si>
+  <si>
+    <t>"PreMIuM"</t>
   </si>
 </sst>
 </file>
@@ -251,57 +425,21 @@
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF067D17"/>
-      <name val="JetBrains Mono"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -316,8 +454,53 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF067D17"/>
+      <name val="JetBrains Mono"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF008000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF067D17"/>
+      <name val="JetBrains Mono"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -336,6 +519,24 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -349,7 +550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -357,19 +558,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,7 +680,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:N44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:N45">
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="I/O"/>
@@ -729,27 +932,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD1001"/>
+  <dimension ref="A1:AD1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.109375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col min="1" max="2" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="30.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="31.28515625" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" customWidth="1"/>
-    <col min="13" max="13" width="70.85546875" customWidth="1"/>
-    <col min="14" max="30" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="31.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="70.88671875" customWidth="1"/>
+    <col min="14" max="30" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="15.75" customHeight="1">
@@ -834,7 +1037,7 @@
       <c r="G2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="16">
         <v>8421691423220</v>
       </c>
       <c r="I2" s="6" t="s">
@@ -844,13 +1047,13 @@
         <v>20</v>
       </c>
       <c r="K2" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="M2" s="6" t="s">
-        <v>23</v>
+        <v>123</v>
       </c>
       <c r="N2" s="4"/>
     </row>
@@ -868,31 +1071,31 @@
         <v>7</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="I3" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K3" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="M3" s="6" t="s">
-        <v>29</v>
+        <v>122</v>
       </c>
       <c r="N3" s="4"/>
     </row>
@@ -910,15 +1113,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="13">
+        <v>27</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="16">
         <v>8421691423225</v>
       </c>
       <c r="I4" s="6" t="s">
@@ -928,13 +1131,13 @@
         <v>20</v>
       </c>
       <c r="K4" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="M4" s="6" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="N4" s="4"/>
     </row>
@@ -948,35 +1151,33 @@
       <c r="C5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>60</v>
+      <c r="E5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="H5" s="16">
+        <v>8421691</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K5" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="M5" s="6" t="s">
-        <v>29</v>
+        <v>120</v>
       </c>
       <c r="N5" s="4"/>
     </row>
@@ -990,24 +1191,34 @@
       <c r="C6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="6"/>
+      <c r="E6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" s="16">
+        <v>8421691423220150</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>121</v>
+      </c>
       <c r="N6" s="4"/>
     </row>
     <row r="7" spans="1:30" ht="15.75" customHeight="1">
@@ -1020,27 +1231,43 @@
       <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="6"/>
+      <c r="D7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="16">
+        <v>8421691423220</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="N7" s="4"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1">
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -1053,28 +1280,28 @@
         <v>16</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="16">
         <v>8421691423220</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>28</v>
+        <v>124</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K8" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="M8" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="N8" s="4"/>
     </row>
@@ -1082,385 +1309,833 @@
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>24</v>
+      <c r="E9" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" s="13">
+        <v>72</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" s="16">
         <v>8421691423220</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K9" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L9" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="M9" s="6" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="N9" s="4"/>
     </row>
-    <row r="10" spans="1:30" ht="16.5" customHeight="1">
+    <row r="10" spans="1:30" ht="15.75" customHeight="1">
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="6"/>
+      <c r="B10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="16">
+        <v>8421691423220</v>
+      </c>
+      <c r="I10" s="6">
+        <v>123</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>114</v>
+      </c>
       <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:30" ht="15.75" customHeight="1">
       <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="6"/>
+      <c r="B11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" s="16">
+        <v>8421691423220</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>115</v>
+      </c>
       <c r="N11" s="4"/>
     </row>
     <row r="12" spans="1:30" ht="15.75" customHeight="1">
       <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="6"/>
+      <c r="B12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="16">
+        <v>8421691423220</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="N12" s="4"/>
     </row>
     <row r="13" spans="1:30" ht="15.75" customHeight="1">
       <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="6"/>
+      <c r="B13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="16">
+        <v>8421691423220</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="N13" s="4"/>
     </row>
     <row r="14" spans="1:30" ht="15.75" customHeight="1">
       <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="6"/>
+      <c r="B14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" s="16">
+        <v>8421691423220</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="6">
+        <v>12345678</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="N14" s="4"/>
     </row>
     <row r="15" spans="1:30" ht="15.75" customHeight="1">
       <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="6"/>
+      <c r="B15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" s="16">
+        <v>8421691423220</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="N15" s="4"/>
     </row>
     <row r="16" spans="1:30" ht="15.75" customHeight="1">
       <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="6"/>
+      <c r="B16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16" s="16">
+        <v>8421691423220</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>71</v>
+      </c>
       <c r="N16" s="4"/>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="6"/>
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="16">
+        <v>8421691423220</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>22</v>
+      </c>
       <c r="N17" s="4"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="6"/>
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" s="16">
+        <v>8421691423220</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>82</v>
+      </c>
       <c r="N18" s="4"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1">
       <c r="A19" s="4">
-        <v>16</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H19" s="16">
+        <v>8421691423220</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M19" s="12" t="s">
+        <v>88</v>
+      </c>
       <c r="N19" s="4"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1">
       <c r="A20" s="4">
-        <v>17</v>
-      </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="6"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H20" s="16">
+        <v>8421691423220</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M20" s="12" t="s">
+        <v>92</v>
+      </c>
       <c r="N20" s="4"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1">
       <c r="A21" s="4">
-        <v>18</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="6"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H21" s="16">
+        <v>8421691423220</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M21" s="12" t="s">
+        <v>95</v>
+      </c>
       <c r="N21" s="4"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1">
       <c r="A22" s="4">
-        <v>19</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H22" s="16">
+        <v>8421691423220</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M22" s="12" t="s">
+        <v>111</v>
+      </c>
       <c r="N22" s="4"/>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1">
       <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="16">
+        <v>8421691423220</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="6"/>
+      <c r="K23" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L23" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="N23" s="4"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1">
       <c r="A24" s="4">
-        <v>21</v>
-      </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="6"/>
+      <c r="G24" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H24" s="16">
+        <v>8421691423220</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L24" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>98</v>
+      </c>
       <c r="N24" s="4"/>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1">
       <c r="A25" s="4">
-        <v>22</v>
-      </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H25" s="16">
+        <v>8421691423220</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L25" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>100</v>
+      </c>
       <c r="N25" s="4"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1">
       <c r="A26" s="4">
-        <v>23</v>
-      </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="6"/>
+      <c r="G26" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H26" s="16">
+        <v>8421691423220</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L26" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="M26" s="6" t="s">
+        <v>102</v>
+      </c>
       <c r="N26" s="4"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1">
       <c r="A27" s="4">
-        <v>24</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H27" s="16">
+        <v>8421691423220</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L27" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="M27" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="N27" s="4"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1">
       <c r="A28" s="4">
-        <v>25</v>
-      </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H28" s="16">
+        <v>8421691423220</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L28" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="M28" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="N28" s="11"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1">
       <c r="A29" s="4">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1472,13 +2147,13 @@
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
-      <c r="L29" s="4"/>
+      <c r="L29" s="14"/>
       <c r="M29" s="6"/>
       <c r="N29" s="4"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1">
       <c r="A30" s="4">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1490,31 +2165,31 @@
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="6"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="15"/>
       <c r="N30" s="4"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1">
       <c r="A31" s="4">
-        <v>28</v>
-      </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
-      <c r="L31" s="4"/>
+      <c r="L31" s="14"/>
       <c r="M31" s="6"/>
       <c r="N31" s="4"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1">
       <c r="A32" s="4">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1522,17 +2197,17 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="6"/>
       <c r="N32" s="4"/>
     </row>
     <row r="33" spans="1:14" ht="15.75" customHeight="1">
       <c r="A33" s="4">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1549,23 +2224,12 @@
       <c r="N33" s="4"/>
     </row>
     <row r="34" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A34" s="4">
-        <v>31</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-      <c r="E34" s="4" t="s">
-        <v>39</v>
-      </c>
+      <c r="E34" s="4"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="4" t="s">
-        <v>40</v>
-      </c>
+      <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
@@ -1575,22 +2239,19 @@
       <c r="N34" s="4"/>
     </row>
     <row r="35" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A35" s="4">
-        <v>32</v>
-      </c>
       <c r="B35" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
@@ -1601,13 +2262,20 @@
       <c r="N35" s="4"/>
     </row>
     <row r="36" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
+      <c r="B36" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
+      <c r="E36" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
+      <c r="G36" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
@@ -1638,9 +2306,7 @@
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
-      <c r="F38" s="15" t="s">
-        <v>64</v>
-      </c>
+      <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
@@ -1656,9 +2322,7 @@
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
-      <c r="F39" s="15" t="s">
-        <v>65</v>
-      </c>
+      <c r="F39" s="4"/>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
@@ -1674,9 +2338,7 @@
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
-      <c r="F40" s="15" t="s">
-        <v>66</v>
-      </c>
+      <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
@@ -1750,7 +2412,22 @@
       <c r="M44" s="4"/>
       <c r="N44" s="4"/>
     </row>
-    <row r="45" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+    </row>
     <row r="46" spans="1:14" ht="15.75" customHeight="1"/>
     <row r="47" spans="1:14" ht="15.75" customHeight="1"/>
     <row r="48" spans="1:14" ht="15.75" customHeight="1"/>
@@ -2707,11 +3384,12 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2720,70 +3398,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="165" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.109375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
-    <col min="4" max="4" width="44.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="62.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" customWidth="1"/>
-    <col min="8" max="8" width="36.7109375" customWidth="1"/>
-    <col min="9" max="10" width="33.7109375" customWidth="1"/>
-    <col min="11" max="28" width="10.5703125" customWidth="1"/>
+    <col min="1" max="2" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" customWidth="1"/>
+    <col min="4" max="4" width="44.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="6" max="6" width="62.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" customWidth="1"/>
+    <col min="8" max="8" width="36.6640625" customWidth="1"/>
+    <col min="9" max="10" width="33.6640625" customWidth="1"/>
+    <col min="11" max="28" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="33" customHeight="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="10" t="s">
+      <c r="B1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" s="10" t="s">
+      <c r="G1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
-      <c r="AB1" s="11"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" customHeight="1">
       <c r="A2" s="4">
@@ -2793,25 +3473,25 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="J2" s="4"/>
     </row>
@@ -4287,15 +4967,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.109375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="62.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" customWidth="1"/>
-    <col min="6" max="7" width="33.7109375" customWidth="1"/>
-    <col min="8" max="25" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="62.33203125" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" customWidth="1"/>
+    <col min="6" max="7" width="33.6640625" customWidth="1"/>
+    <col min="8" max="25" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1">
@@ -4303,7 +4983,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>5</v>
@@ -4312,10 +4992,10 @@
         <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>13</v>
@@ -4326,11 +5006,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>

</xml_diff>

<commit_message>
Added All the Excel (first function)
</commit_message>
<xml_diff>
--- a/docs/GE3_TestCasesTemplate_2023_v1.0.xlsx
+++ b/docs/GE3_TestCasesTemplate_2023_v1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\OneDrive\Escritorio\Desarrollo de Software\G89.2023.T20.EG3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edu/PycharmProjects/G89.2023.T20.EG3/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922B4995-BA05-45C2-A004-3B4754C13E53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFDF80A-EA87-B04D-B311-742378C84168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="1515" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="500" windowWidth="27720" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GE3 2023 F1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="148">
   <si>
     <t>#</t>
   </si>
@@ -104,9 +104,6 @@
     <t>CE_NV_2</t>
   </si>
   <si>
-    <t>842169142322A</t>
-  </si>
-  <si>
     <t>"PREMIUM"</t>
   </si>
   <si>
@@ -117,18 +114,6 @@
   </si>
   <si>
     <t>OUTPUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valid </t>
-  </si>
-  <si>
-    <t xml:space="preserve">add a regular and a family </t>
-  </si>
-  <si>
-    <t xml:space="preserve">valid </t>
-  </si>
-  <si>
-    <t>add a regular and 2 family</t>
   </si>
   <si>
     <t>NODE</t>
@@ -187,15 +172,9 @@
     <t>"regular"</t>
   </si>
   <si>
-    <t>"premiums"</t>
-  </si>
-  <si>
     <t>PRODUCT ID NOT (EA13)NUMBER</t>
   </si>
   <si>
-    <t>"regula"</t>
-  </si>
-  <si>
     <t>ORDER_TYPE NOT VALID (not a string)</t>
   </si>
   <si>
@@ -244,9 +223,6 @@
     <t>ADDRES_LENGTH BIG</t>
   </si>
   <si>
-    <t xml:space="preserve">"CALLE DE NUESTRO SEÑOR SATORU GOJO EL BENEVOLENTE QUE CON SUS ARTES MARCIALES Y SU ESPECIAL AURA MURIÓ, MADRID, ESPAÑA"  </t>
-  </si>
-  <si>
     <t>Exception: Address too long</t>
   </si>
   <si>
@@ -256,24 +232,12 @@
     <t>CE_NV_9</t>
   </si>
   <si>
-    <t>CE_NV_10</t>
-  </si>
-  <si>
-    <t>CE_V_5</t>
-  </si>
-  <si>
     <t>CE_V_6</t>
   </si>
   <si>
     <t>PHONE_NUMBER_TYPE NOT VALID</t>
   </si>
   <si>
-    <t>ORDER_TYPE NOT VALID TOO LONG</t>
-  </si>
-  <si>
-    <t>ORDER_TYPE NOT VALID TOO SHORT</t>
-  </si>
-  <si>
     <t>CE_V_17</t>
   </si>
   <si>
@@ -301,24 +265,15 @@
     <t>¿Valid Phone number?</t>
   </si>
   <si>
-    <t>CE_NV_XX</t>
-  </si>
-  <si>
     <t>PHONE_NUMBER TOO SHORT</t>
   </si>
   <si>
-    <t>"123456"</t>
-  </si>
-  <si>
     <t>Exception: Phone_number too short</t>
   </si>
   <si>
     <t>PHONE_NUMBER TOO LONG</t>
   </si>
   <si>
-    <t>"123456789123456"</t>
-  </si>
-  <si>
     <t>Exception: Phone_number too long</t>
   </si>
   <si>
@@ -340,48 +295,18 @@
     <t>ZIP_CODE TOO FEW DIGITS</t>
   </si>
   <si>
-    <t>Exception: Zip_Code too few digits</t>
-  </si>
-  <si>
     <t>ZIP_CODE NON INTEGER VALUE</t>
   </si>
   <si>
     <t>Exception: Zip_Code must be an integer {01000-52999}</t>
   </si>
   <si>
-    <t>"942"</t>
-  </si>
-  <si>
-    <t>"53942"</t>
-  </si>
-  <si>
-    <t>"2382"</t>
-  </si>
-  <si>
     <t>"La casa de paco"</t>
   </si>
   <si>
-    <t>ZIP_CODE FLOAT VALUE</t>
-  </si>
-  <si>
-    <t>"23.82"</t>
-  </si>
-  <si>
-    <t>Exception: Phone_number is not of type FLOAT</t>
-  </si>
-  <si>
-    <t>"123456.789123456"</t>
-  </si>
-  <si>
-    <t>Exception: Order Type Value too long</t>
-  </si>
-  <si>
     <t>Exception: Order Type value is not a string</t>
   </si>
   <si>
-    <t>Exception: Order Type Value too short</t>
-  </si>
-  <si>
     <t>"654314159"</t>
   </si>
   <si>
@@ -406,14 +331,158 @@
     <t>e01521684a7f9535e9fa098a2b86565f</t>
   </si>
   <si>
-    <t>"PreMIuM"</t>
+    <t>VL</t>
+  </si>
+  <si>
+    <t>CE_NV_4</t>
+  </si>
+  <si>
+    <t>CE_NV_5</t>
+  </si>
+  <si>
+    <t>CE_V_10</t>
+  </si>
+  <si>
+    <t>ORDER_TYPE VALID</t>
+  </si>
+  <si>
+    <t>"premium"</t>
+  </si>
+  <si>
+    <t>ORDER_TYPE NOT UPPER_CASE</t>
+  </si>
+  <si>
+    <t>ADDRES_TWO_SPACES</t>
+  </si>
+  <si>
+    <t>ADDRES_ONE_SPACE</t>
+  </si>
+  <si>
+    <t>"C/LISBOA MARINERA,4, MADRID, SPAIN"</t>
+  </si>
+  <si>
+    <t>CALLE DE NUESTRO SEÑOR SATORU GOJO EL BENEVOLENTE QUE CON SUS ARTES MARCIALES NATURAL, MADRID, ESPAÑA</t>
+  </si>
+  <si>
+    <t>LV</t>
+  </si>
+  <si>
+    <t>CE_V_11</t>
+  </si>
+  <si>
+    <t>ADDRES CORRECT</t>
+  </si>
+  <si>
+    <t>PHONE_NUMBER EXACT SIZE</t>
+  </si>
+  <si>
+    <t>CE_NV_20</t>
+  </si>
+  <si>
+    <t>CE_NV_21</t>
+  </si>
+  <si>
+    <t>CE_NV_22</t>
+  </si>
+  <si>
+    <t>"65431415"</t>
+  </si>
+  <si>
+    <t>ZIP_CODE TOO MANY DIGITS</t>
+  </si>
+  <si>
+    <t>"00999"</t>
+  </si>
+  <si>
+    <t>"53000"</t>
+  </si>
+  <si>
+    <t>"520000"</t>
+  </si>
+  <si>
+    <t>"0011"</t>
+  </si>
+  <si>
+    <t>"6942069420"</t>
+  </si>
+  <si>
+    <t>"8421691423220"</t>
+  </si>
+  <si>
+    <t>"84216914232202"</t>
+  </si>
+  <si>
+    <t>"842169142322"</t>
+  </si>
+  <si>
+    <t>"842169142322A"</t>
+  </si>
+  <si>
+    <t>FILE DOES NOT EXIST</t>
+  </si>
+  <si>
+    <t>FILE WRONG STRCUTRE</t>
+  </si>
+  <si>
+    <t>FILE IS NOT MODIFIED AS INVALID INPUT</t>
+  </si>
+  <si>
+    <t>FILE IS CORRECT</t>
+  </si>
+  <si>
+    <t>OUTPUT FILE</t>
+  </si>
+  <si>
+    <t>¿?¿?</t>
+  </si>
+  <si>
+    <t>"84216914232"</t>
+  </si>
+  <si>
+    <t>CE_V_23</t>
+  </si>
+  <si>
+    <t>CE_NV_24</t>
+  </si>
+  <si>
+    <t>CE_NV_25</t>
+  </si>
+  <si>
+    <t>CE_NV_26</t>
+  </si>
+  <si>
+    <t>CE_NV_27</t>
+  </si>
+  <si>
+    <t>CE_NV_28</t>
+  </si>
+  <si>
+    <t>CE_NV_29</t>
+  </si>
+  <si>
+    <t>CE_NV_30</t>
+  </si>
+  <si>
+    <t>CE_NV_31</t>
+  </si>
+  <si>
+    <t>CE_NV_32</t>
+  </si>
+  <si>
+    <t>CE_V_7</t>
+  </si>
+  <si>
+    <t>Exception: Zip_Code has too many digits</t>
+  </si>
+  <si>
+    <t>Exception: Zip_Code has too few digits</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="13">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -460,19 +529,6 @@
       <name val="JetBrains Mono"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="0"/>
@@ -492,12 +548,6 @@
       <color rgb="FF008000"/>
       <name val="Helvetica"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FF067D17"/>
-      <name val="JetBrains Mono"/>
     </font>
   </fonts>
   <fills count="7">
@@ -550,7 +600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -560,18 +610,18 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -680,7 +730,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:N45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:N47">
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="I/O"/>
@@ -932,27 +982,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD1002"/>
+  <dimension ref="A1:AD1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="7" ySplit="19" topLeftCell="K20" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.109375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="10.5546875" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="30.33203125" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="31.33203125" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" customWidth="1"/>
-    <col min="13" max="13" width="70.88671875" customWidth="1"/>
-    <col min="14" max="30" width="10.5546875" customWidth="1"/>
+    <col min="10" max="10" width="47.7109375" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="30" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="15.75" customHeight="1">
@@ -1037,8 +1091,8 @@
       <c r="G2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="16">
-        <v>8421691423220</v>
+      <c r="H2" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>19</v>
@@ -1047,13 +1101,13 @@
         <v>20</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L2" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="L2" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="N2" s="4"/>
     </row>
@@ -1077,25 +1131,25 @@
         <v>24</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H3" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L3" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="L3" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="N3" s="4"/>
     </row>
@@ -1116,13 +1170,13 @@
         <v>23</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="16">
-        <v>8421691423225</v>
+      <c r="H4" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>19</v>
@@ -1131,13 +1185,13 @@
         <v>20</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L4" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="L4" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="N4" s="4"/>
     </row>
@@ -1149,7 +1203,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>7</v>
@@ -1157,12 +1211,14 @@
       <c r="E5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="G5" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="H5" s="16">
-        <v>8421691</v>
+        <v>92</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>126</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>19</v>
@@ -1171,13 +1227,13 @@
         <v>20</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L5" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="L5" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="N5" s="4"/>
     </row>
@@ -1189,7 +1245,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>7</v>
@@ -1197,12 +1253,14 @@
       <c r="E6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>101</v>
+      </c>
       <c r="G6" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H6" s="16">
-        <v>8421691423220150</v>
+        <v>93</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>125</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>19</v>
@@ -1211,13 +1269,13 @@
         <v>20</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L6" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="L6" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="N6" s="4"/>
     </row>
@@ -1238,24 +1296,24 @@
         <v>16</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="16">
-        <v>8421691423220</v>
+        <v>103</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L7" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="L7" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M7" s="6" t="s">
@@ -1280,24 +1338,24 @@
         <v>16</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>76</v>
+        <v>145</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="16">
-        <v>8421691423220</v>
+        <v>103</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L8" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="L8" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M8" s="6" t="s">
@@ -1322,28 +1380,28 @@
         <v>23</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H9" s="16">
-        <v>8421691423220</v>
+        <v>105</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L9" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="L9" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>113</v>
+        <v>22</v>
       </c>
       <c r="N9" s="4"/>
     </row>
@@ -1364,13 +1422,13 @@
         <v>23</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" s="16">
-        <v>8421691423220</v>
+        <v>47</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I10" s="6">
         <v>123</v>
@@ -1379,19 +1437,19 @@
         <v>20</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L10" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="L10" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:30" ht="15.75" customHeight="1">
       <c r="A11" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>14</v>
@@ -1400,77 +1458,65 @@
         <v>15</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="H11" s="16">
-        <v>8421691423220</v>
+        <v>112</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L11" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="K11" s="6"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="6"/>
       <c r="N11" s="4"/>
     </row>
     <row r="12" spans="1:30" ht="15.75" customHeight="1">
       <c r="A12" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>56</v>
+        <v>111</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="16">
-        <v>8421691423220</v>
+        <v>106</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>19</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L12" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>22</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="K12" s="6"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="6"/>
       <c r="N12" s="4"/>
     </row>
     <row r="13" spans="1:30" ht="15.75" customHeight="1">
@@ -1481,37 +1527,37 @@
         <v>14</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H13" s="16">
-        <v>8421691423220</v>
+        <v>107</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>19</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L13" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="L13" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="N13" s="4"/>
     </row>
@@ -1523,37 +1569,37 @@
         <v>14</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H14" s="16">
-        <v>8421691423220</v>
+        <v>51</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="6">
-        <v>12345678</v>
+      <c r="J14" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L14" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="L14" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="N14" s="4"/>
     </row>
@@ -1568,34 +1614,34 @@
         <v>15</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H15" s="16">
-        <v>8421691423220</v>
+        <v>55</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="6" t="s">
-        <v>66</v>
+      <c r="J15" s="6">
+        <v>12345678</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L15" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="L15" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="N15" s="4"/>
     </row>
@@ -1607,37 +1653,37 @@
         <v>14</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="H16" s="16">
-        <v>8421691423220</v>
+        <v>58</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>19</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L16" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="L16" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="N16" s="4"/>
     </row>
@@ -1648,38 +1694,38 @@
       <c r="B17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="4" t="s">
+      <c r="C17" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>80</v>
+      <c r="F17" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="16">
-        <v>8421691423220</v>
+        <v>62</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>109</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L17" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="L17" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="M17" s="12" t="s">
-        <v>22</v>
+      <c r="M17" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="N17" s="4"/>
     </row>
@@ -1700,28 +1746,28 @@
         <v>23</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H18" s="16">
-        <v>8421691423220</v>
+        <v>18</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="L18" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="L18" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="M18" s="12" t="s">
-        <v>82</v>
+      <c r="M18" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="N18" s="4"/>
     </row>
@@ -1739,31 +1785,31 @@
         <v>10</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="H19" s="16">
-        <v>8421691423220</v>
+        <v>67</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="J19" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="L19" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="L19" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="M19" s="12" t="s">
-        <v>88</v>
+      <c r="M19" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="N19" s="4"/>
     </row>
@@ -1781,31 +1827,31 @@
         <v>10</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="H20" s="16">
-        <v>8421691423220</v>
+        <v>75</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="J20" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="L20" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="L20" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="M20" s="12" t="s">
-        <v>92</v>
+      <c r="M20" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="N20" s="4"/>
     </row>
@@ -1817,7 +1863,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>10</v>
@@ -1826,28 +1872,28 @@
         <v>23</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="H21" s="16">
-        <v>8421691423220</v>
+        <v>77</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="J21" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="L21" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="L21" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="M21" s="12" t="s">
-        <v>95</v>
+      <c r="M21" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="N21" s="4"/>
     </row>
@@ -1859,7 +1905,7 @@
         <v>14</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>10</v>
@@ -1868,28 +1914,28 @@
         <v>23</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="H22" s="16">
-        <v>8421691423220</v>
+        <v>79</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="J22" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="L22" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="L22" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="M22" s="12" t="s">
-        <v>111</v>
+      <c r="M22" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="N22" s="4"/>
     </row>
@@ -1901,31 +1947,33 @@
         <v>14</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="G23" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="16">
-        <v>8421691423220</v>
+        <v>113</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="J23" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L23" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="L23" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M23" s="6" t="s">
@@ -1937,7 +1985,7 @@
       <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -1947,14 +1995,16 @@
         <v>11</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F24" s="4"/>
+        <v>16</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="G24" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="H24" s="16">
-        <v>8421691423220</v>
+        <v>18</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>19</v>
@@ -1963,13 +2013,13 @@
         <v>20</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L24" s="12" t="s">
-        <v>105</v>
+        <v>91</v>
+      </c>
+      <c r="L24" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>98</v>
+        <v>22</v>
       </c>
       <c r="N24" s="4"/>
     </row>
@@ -1980,21 +2030,23 @@
       <c r="B25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>15</v>
+      <c r="C25" s="4" t="s">
+        <v>110</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="H25" s="16">
-        <v>8421691423220</v>
+      <c r="E25" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>19</v>
@@ -2003,13 +2055,13 @@
         <v>20</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L25" s="12" t="s">
-        <v>106</v>
+        <v>91</v>
+      </c>
+      <c r="L25" s="11" t="s">
+        <v>119</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="N25" s="4"/>
     </row>
@@ -2021,20 +2073,22 @@
         <v>14</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F26" s="4"/>
+        <v>81</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>137</v>
+      </c>
       <c r="G26" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H26" s="16">
-        <v>8421691423220</v>
+        <v>84</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>19</v>
@@ -2043,13 +2097,13 @@
         <v>20</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L26" s="12" t="s">
-        <v>107</v>
+        <v>91</v>
+      </c>
+      <c r="L26" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="N26" s="4"/>
     </row>
@@ -2061,20 +2115,22 @@
         <v>14</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F27" s="4"/>
+        <v>81</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="G27" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H27" s="16">
-        <v>8421691423220</v>
+        <v>118</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>19</v>
@@ -2083,13 +2139,13 @@
         <v>20</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L27" s="12" t="s">
-        <v>108</v>
+        <v>91</v>
+      </c>
+      <c r="L27" s="11" t="s">
+        <v>121</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>104</v>
+        <v>146</v>
       </c>
       <c r="N27" s="4"/>
     </row>
@@ -2101,20 +2157,22 @@
         <v>14</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F28" s="4"/>
+        <v>81</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="G28" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="H28" s="16">
-        <v>8421691423220</v>
+        <v>86</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>19</v>
@@ -2123,104 +2181,224 @@
         <v>20</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L28" s="12" t="s">
-        <v>110</v>
+        <v>91</v>
+      </c>
+      <c r="L28" s="11" t="s">
+        <v>122</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="N28" s="11"/>
+        <v>147</v>
+      </c>
+      <c r="N28" s="4"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1">
       <c r="A29" s="4">
         <v>28</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="6"/>
+      <c r="B29" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="L29" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="N29" s="4"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1">
       <c r="A30" s="4">
         <v>29</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="4"/>
+      <c r="B30" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="L30" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M30" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="N30" s="9"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1">
       <c r="A31" s="4">
         <v>30</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="6"/>
+      <c r="B31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="L31" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>133</v>
+      </c>
       <c r="N31" s="4"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1">
       <c r="A32" s="4">
         <v>31</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="6"/>
+      <c r="B32" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="L32" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>133</v>
+      </c>
       <c r="N32" s="4"/>
     </row>
     <row r="33" spans="1:14" ht="15.75" customHeight="1">
       <c r="A33" s="4">
         <v>32</v>
       </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
+      <c r="B33" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="L33" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M33" s="6" t="s">
+        <v>133</v>
+      </c>
       <c r="N33" s="4"/>
     </row>
     <row r="34" spans="1:14" ht="15.75" customHeight="1">
@@ -2230,29 +2408,21 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="6"/>
       <c r="N34" s="4"/>
     </row>
     <row r="35" spans="1:14" ht="15.75" customHeight="1">
-      <c r="B35" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="4" t="s">
-        <v>30</v>
-      </c>
+      <c r="E35" s="4"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
@@ -2262,20 +2432,12 @@
       <c r="N35" s="4"/>
     </row>
     <row r="36" spans="1:14" ht="15.75" customHeight="1">
-      <c r="B36" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-      <c r="E36" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="E36" s="4"/>
       <c r="F36" s="4"/>
-      <c r="G36" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
@@ -2285,7 +2447,6 @@
       <c r="N36" s="4"/>
     </row>
     <row r="37" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
@@ -2301,7 +2462,6 @@
       <c r="N37" s="4"/>
     </row>
     <row r="38" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -2428,8 +2588,38 @@
       <c r="M45" s="4"/>
       <c r="N45" s="4"/>
     </row>
-    <row r="46" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="47" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+    </row>
+    <row r="47" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+    </row>
     <row r="48" spans="1:14" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
@@ -3385,6 +3575,8 @@
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
     <row r="1002" ht="15.75" customHeight="1"/>
+    <row r="1003" ht="15.75" customHeight="1"/>
+    <row r="1004" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -3402,68 +3594,68 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.109375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="10.5546875" customWidth="1"/>
-    <col min="3" max="3" width="26.5546875" customWidth="1"/>
-    <col min="4" max="4" width="44.109375" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" customWidth="1"/>
-    <col min="6" max="6" width="62.33203125" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" customWidth="1"/>
-    <col min="8" max="8" width="36.6640625" customWidth="1"/>
-    <col min="9" max="10" width="33.6640625" customWidth="1"/>
-    <col min="11" max="28" width="10.5546875" customWidth="1"/>
+    <col min="1" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="44.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="6" max="6" width="62.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" customWidth="1"/>
+    <col min="8" max="8" width="36.7109375" customWidth="1"/>
+    <col min="9" max="10" width="33.7109375" customWidth="1"/>
+    <col min="11" max="28" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="33" customHeight="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" customHeight="1">
       <c r="A2" s="4">
@@ -3473,25 +3665,25 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="J2" s="4"/>
     </row>
@@ -4967,15 +5159,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.109375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="62.33203125" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" customWidth="1"/>
-    <col min="6" max="7" width="33.6640625" customWidth="1"/>
-    <col min="8" max="25" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="62.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" customWidth="1"/>
+    <col min="6" max="7" width="33.7109375" customWidth="1"/>
+    <col min="8" max="25" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1">
@@ -4983,7 +5175,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>5</v>
@@ -4992,10 +5184,10 @@
         <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>13</v>
@@ -5006,11 +5198,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>

</xml_diff>

<commit_message>
Modified until test 8
</commit_message>
<xml_diff>
--- a/docs/GE3_TestCasesTemplate_2023_v1.0.xlsx
+++ b/docs/GE3_TestCasesTemplate_2023_v1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edu/PycharmProjects/G89.2023.T20.EG3/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFDF80A-EA87-B04D-B311-742378C84168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3494A78C-A4EC-474A-8AC2-4F2776393809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="500" windowWidth="27720" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="149">
   <si>
     <t>#</t>
   </si>
@@ -304,9 +304,6 @@
     <t>"La casa de paco"</t>
   </si>
   <si>
-    <t>Exception: Order Type value is not a string</t>
-  </si>
-  <si>
     <t>"654314159"</t>
   </si>
   <si>
@@ -476,6 +473,12 @@
   </si>
   <si>
     <t>Exception: Zip_Code has too few digits</t>
+  </si>
+  <si>
+    <t>Exception: Order type not valid, must be REGULAR or PREMIUM</t>
+  </si>
+  <si>
+    <t>Exception: Type of the order_type is not valid, must be a STRING</t>
   </si>
 </sst>
 </file>
@@ -988,7 +991,7 @@
       <pane xSplit="7" ySplit="19" topLeftCell="K20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="M30" sqref="M30"/>
+      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="15" customHeight="1"/>
@@ -1005,7 +1008,7 @@
     <col min="10" max="10" width="47.7109375" customWidth="1"/>
     <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="52.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="30" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1092,7 +1095,7 @@
         <v>18</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>19</v>
@@ -1101,13 +1104,13 @@
         <v>20</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L2" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N2" s="4"/>
     </row>
@@ -1134,7 +1137,7 @@
         <v>46</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>25</v>
@@ -1143,13 +1146,13 @@
         <v>20</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L3" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N3" s="4"/>
     </row>
@@ -1176,7 +1179,7 @@
         <v>27</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>19</v>
@@ -1185,13 +1188,13 @@
         <v>20</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L4" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N4" s="4"/>
     </row>
@@ -1203,7 +1206,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>7</v>
@@ -1212,13 +1215,13 @@
         <v>23</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>19</v>
@@ -1227,13 +1230,13 @@
         <v>20</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L5" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N5" s="4"/>
     </row>
@@ -1245,7 +1248,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>7</v>
@@ -1254,13 +1257,13 @@
         <v>23</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>19</v>
@@ -1269,13 +1272,13 @@
         <v>20</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L6" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N6" s="4"/>
     </row>
@@ -1299,10 +1302,10 @@
         <v>66</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>19</v>
@@ -1311,7 +1314,7 @@
         <v>20</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L7" s="11" t="s">
         <v>21</v>
@@ -1338,13 +1341,13 @@
         <v>16</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>25</v>
@@ -1353,7 +1356,7 @@
         <v>20</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L8" s="11" t="s">
         <v>21</v>
@@ -1383,25 +1386,25 @@
         <v>64</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L9" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>22</v>
+        <v>147</v>
       </c>
       <c r="N9" s="4"/>
     </row>
@@ -1428,7 +1431,7 @@
         <v>47</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I10" s="6">
         <v>123</v>
@@ -1437,13 +1440,13 @@
         <v>20</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L10" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>90</v>
+        <v>148</v>
       </c>
       <c r="N10" s="4"/>
     </row>
@@ -1464,13 +1467,13 @@
         <v>16</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>19</v>
@@ -1491,7 +1494,7 @@
         <v>14</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>48</v>
@@ -1500,19 +1503,19 @@
         <v>16</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>19</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="11"/>
@@ -1527,7 +1530,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>48</v>
@@ -1539,10 +1542,10 @@
         <v>49</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>19</v>
@@ -1551,7 +1554,7 @@
         <v>20</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L13" s="11" t="s">
         <v>21</v>
@@ -1569,7 +1572,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>48</v>
@@ -1584,7 +1587,7 @@
         <v>51</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>19</v>
@@ -1593,7 +1596,7 @@
         <v>52</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L14" s="11" t="s">
         <v>21</v>
@@ -1626,7 +1629,7 @@
         <v>55</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>19</v>
@@ -1635,7 +1638,7 @@
         <v>12345678</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L15" s="11" t="s">
         <v>21</v>
@@ -1653,7 +1656,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>48</v>
@@ -1668,7 +1671,7 @@
         <v>58</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>19</v>
@@ -1677,7 +1680,7 @@
         <v>59</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L16" s="11" t="s">
         <v>21</v>
@@ -1695,7 +1698,7 @@
         <v>14</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>48</v>
@@ -1710,16 +1713,16 @@
         <v>62</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>19</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L17" s="11" t="s">
         <v>21</v>
@@ -1752,7 +1755,7 @@
         <v>18</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>45</v>
@@ -1761,7 +1764,7 @@
         <v>20</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L18" s="11" t="s">
         <v>21</v>
@@ -1794,7 +1797,7 @@
         <v>67</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>45</v>
@@ -1836,7 +1839,7 @@
         <v>75</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>45</v>
@@ -1863,7 +1866,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>10</v>
@@ -1872,13 +1875,13 @@
         <v>23</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>77</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>45</v>
@@ -1887,7 +1890,7 @@
         <v>20</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L21" s="11" t="s">
         <v>21</v>
@@ -1905,7 +1908,7 @@
         <v>14</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>10</v>
@@ -1914,13 +1917,13 @@
         <v>23</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>79</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>45</v>
@@ -1929,7 +1932,7 @@
         <v>20</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L22" s="11" t="s">
         <v>21</v>
@@ -1947,7 +1950,7 @@
         <v>14</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>10</v>
@@ -1956,13 +1959,13 @@
         <v>23</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>45</v>
@@ -1971,7 +1974,7 @@
         <v>20</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L23" s="11" t="s">
         <v>21</v>
@@ -1998,13 +2001,13 @@
         <v>16</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>18</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>19</v>
@@ -2013,7 +2016,7 @@
         <v>20</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L24" s="11" t="s">
         <v>21</v>
@@ -2031,7 +2034,7 @@
         <v>14</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>11</v>
@@ -2040,13 +2043,13 @@
         <v>81</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>82</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>19</v>
@@ -2055,10 +2058,10 @@
         <v>20</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L25" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M25" s="6" t="s">
         <v>83</v>
@@ -2073,7 +2076,7 @@
         <v>14</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>11</v>
@@ -2082,13 +2085,13 @@
         <v>81</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>84</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>19</v>
@@ -2097,10 +2100,10 @@
         <v>20</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L26" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M26" s="6" t="s">
         <v>85</v>
@@ -2115,7 +2118,7 @@
         <v>14</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>11</v>
@@ -2124,13 +2127,13 @@
         <v>81</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>19</v>
@@ -2139,13 +2142,13 @@
         <v>20</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L27" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N27" s="4"/>
     </row>
@@ -2157,7 +2160,7 @@
         <v>14</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>11</v>
@@ -2166,13 +2169,13 @@
         <v>81</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>86</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>19</v>
@@ -2181,13 +2184,13 @@
         <v>20</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L28" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N28" s="4"/>
     </row>
@@ -2208,13 +2211,13 @@
         <v>81</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>87</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I29" s="6" t="s">
         <v>19</v>
@@ -2223,7 +2226,7 @@
         <v>20</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L29" s="11" t="s">
         <v>89</v>
@@ -2244,19 +2247,19 @@
         <v>15</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>81</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I30" s="6" t="s">
         <v>19</v>
@@ -2265,13 +2268,13 @@
         <v>20</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L30" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N30" s="9"/>
     </row>
@@ -2286,19 +2289,19 @@
         <v>15</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>81</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I31" s="6" t="s">
         <v>19</v>
@@ -2307,13 +2310,13 @@
         <v>20</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L31" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N31" s="4"/>
     </row>
@@ -2328,19 +2331,19 @@
         <v>15</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>81</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>19</v>
@@ -2349,13 +2352,13 @@
         <v>20</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L32" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N32" s="4"/>
     </row>
@@ -2370,19 +2373,19 @@
         <v>15</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I33" s="6" t="s">
         <v>19</v>
@@ -2391,13 +2394,13 @@
         <v>20</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L33" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N33" s="4"/>
     </row>

</xml_diff>

<commit_message>
Created tests and exceptions until 17 - Valid phone number
</commit_message>
<xml_diff>
--- a/docs/GE3_TestCasesTemplate_2023_v1.0.xlsx
+++ b/docs/GE3_TestCasesTemplate_2023_v1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edu/PycharmProjects/G89.2023.T20.EG3/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3494A78C-A4EC-474A-8AC2-4F2776393809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30193AE-89D6-D149-AADB-CF3A82E52EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="500" windowWidth="27720" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="150">
   <si>
     <t>#</t>
   </si>
@@ -193,18 +193,12 @@
     <t>"C/LISBOA4MADRIDSPAIN"</t>
   </si>
   <si>
-    <t>Exception: Addres must contain a space</t>
-  </si>
-  <si>
     <t>CE_NV_14</t>
   </si>
   <si>
     <t>ADDRES_TYPE WRONG</t>
   </si>
   <si>
-    <t>Exception: Address type must by str</t>
-  </si>
-  <si>
     <t>CE_NV_15</t>
   </si>
   <si>
@@ -214,18 +208,12 @@
     <t>"MICASA, MADRID"</t>
   </si>
   <si>
-    <t>Exception: Address too short</t>
-  </si>
-  <si>
     <t>CE_NV_16</t>
   </si>
   <si>
     <t>ADDRES_LENGTH BIG</t>
   </si>
   <si>
-    <t>Exception: Address too long</t>
-  </si>
-  <si>
     <t>CE_NV_8</t>
   </si>
   <si>
@@ -479,6 +467,21 @@
   </si>
   <si>
     <t>Exception: Type of the order_type is not valid, must be a STRING</t>
+  </si>
+  <si>
+    <t>Exception: Address not valid, must have more than 20 characters</t>
+  </si>
+  <si>
+    <t>Exception: Address not valid, must be a string</t>
+  </si>
+  <si>
+    <t>Exception: Address not valid, must have a space</t>
+  </si>
+  <si>
+    <t>Exception: Address not valid, must have less than 100 characters</t>
+  </si>
+  <si>
+    <t>VALID PHONE NUMBER</t>
   </si>
 </sst>
 </file>
@@ -987,11 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="7" ySplit="19" topLeftCell="K20" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="163" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="15" customHeight="1"/>
@@ -1095,7 +1095,7 @@
         <v>18</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>19</v>
@@ -1104,13 +1104,13 @@
         <v>20</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L2" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="N2" s="4"/>
     </row>
@@ -1137,7 +1137,7 @@
         <v>46</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>25</v>
@@ -1146,13 +1146,13 @@
         <v>20</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L3" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="N3" s="4"/>
     </row>
@@ -1179,7 +1179,7 @@
         <v>27</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>19</v>
@@ -1188,13 +1188,13 @@
         <v>20</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L4" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="N4" s="4"/>
     </row>
@@ -1206,7 +1206,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>7</v>
@@ -1215,13 +1215,13 @@
         <v>23</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>19</v>
@@ -1230,13 +1230,13 @@
         <v>20</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L5" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="N5" s="4"/>
     </row>
@@ -1248,7 +1248,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>7</v>
@@ -1257,13 +1257,13 @@
         <v>23</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>19</v>
@@ -1272,13 +1272,13 @@
         <v>20</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L6" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="N6" s="4"/>
     </row>
@@ -1299,13 +1299,13 @@
         <v>16</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>19</v>
@@ -1314,7 +1314,7 @@
         <v>20</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L7" s="11" t="s">
         <v>21</v>
@@ -1341,13 +1341,13 @@
         <v>16</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>25</v>
@@ -1356,7 +1356,7 @@
         <v>20</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L8" s="11" t="s">
         <v>21</v>
@@ -1383,28 +1383,28 @@
         <v>23</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L9" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="N9" s="4"/>
     </row>
@@ -1425,13 +1425,13 @@
         <v>23</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>47</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I10" s="6">
         <v>123</v>
@@ -1440,13 +1440,13 @@
         <v>20</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L10" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="N10" s="4"/>
     </row>
@@ -1467,13 +1467,13 @@
         <v>16</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>19</v>
@@ -1494,7 +1494,7 @@
         <v>14</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>48</v>
@@ -1503,19 +1503,19 @@
         <v>16</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>19</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="11"/>
@@ -1530,7 +1530,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>48</v>
@@ -1542,10 +1542,10 @@
         <v>49</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>19</v>
@@ -1554,7 +1554,7 @@
         <v>20</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L13" s="11" t="s">
         <v>21</v>
@@ -1572,7 +1572,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>48</v>
@@ -1587,7 +1587,7 @@
         <v>51</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>19</v>
@@ -1596,13 +1596,13 @@
         <v>52</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L14" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>53</v>
+        <v>147</v>
       </c>
       <c r="N14" s="4"/>
     </row>
@@ -1623,13 +1623,13 @@
         <v>23</v>
       </c>
       <c r="F15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="H15" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>19</v>
@@ -1638,13 +1638,13 @@
         <v>12345678</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L15" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>56</v>
+        <v>146</v>
       </c>
       <c r="N15" s="4"/>
     </row>
@@ -1656,7 +1656,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>48</v>
@@ -1665,32 +1665,32 @@
         <v>23</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>19</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L16" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>60</v>
+        <v>145</v>
       </c>
       <c r="N16" s="4"/>
     </row>
-    <row r="17" spans="1:14" ht="15.75" customHeight="1">
+    <row r="17" spans="1:14" ht="51" customHeight="1">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>14</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>48</v>
@@ -1707,28 +1707,28 @@
         <v>23</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>19</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L17" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>63</v>
+        <v>148</v>
       </c>
       <c r="N17" s="4"/>
     </row>
@@ -1749,13 +1749,13 @@
         <v>23</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>18</v>
+        <v>149</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>45</v>
@@ -1764,7 +1764,7 @@
         <v>20</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L18" s="11" t="s">
         <v>21</v>
@@ -1791,13 +1791,13 @@
         <v>23</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>45</v>
@@ -1806,13 +1806,13 @@
         <v>20</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="L19" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="N19" s="4"/>
     </row>
@@ -1830,16 +1830,16 @@
         <v>10</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>45</v>
@@ -1848,13 +1848,13 @@
         <v>20</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="L20" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="N20" s="4"/>
     </row>
@@ -1866,7 +1866,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>10</v>
@@ -1875,13 +1875,13 @@
         <v>23</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>45</v>
@@ -1890,13 +1890,13 @@
         <v>20</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="L21" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M21" s="10" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="N21" s="4"/>
     </row>
@@ -1908,7 +1908,7 @@
         <v>14</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>10</v>
@@ -1917,13 +1917,13 @@
         <v>23</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>45</v>
@@ -1932,13 +1932,13 @@
         <v>20</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L22" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M22" s="10" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="N22" s="4"/>
     </row>
@@ -1950,7 +1950,7 @@
         <v>14</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>10</v>
@@ -1959,13 +1959,13 @@
         <v>23</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>45</v>
@@ -1974,7 +1974,7 @@
         <v>20</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L23" s="11" t="s">
         <v>21</v>
@@ -2001,13 +2001,13 @@
         <v>16</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>18</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>19</v>
@@ -2016,7 +2016,7 @@
         <v>20</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L24" s="11" t="s">
         <v>21</v>
@@ -2034,22 +2034,22 @@
         <v>14</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>19</v>
@@ -2058,13 +2058,13 @@
         <v>20</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L25" s="11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="N25" s="4"/>
     </row>
@@ -2076,22 +2076,22 @@
         <v>14</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>19</v>
@@ -2100,13 +2100,13 @@
         <v>20</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L26" s="11" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="N26" s="4"/>
     </row>
@@ -2118,22 +2118,22 @@
         <v>14</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>19</v>
@@ -2142,13 +2142,13 @@
         <v>20</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L27" s="11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="N27" s="4"/>
     </row>
@@ -2160,22 +2160,22 @@
         <v>14</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>19</v>
@@ -2184,13 +2184,13 @@
         <v>20</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L28" s="11" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="N28" s="4"/>
     </row>
@@ -2208,16 +2208,16 @@
         <v>11</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I29" s="6" t="s">
         <v>19</v>
@@ -2226,13 +2226,13 @@
         <v>20</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L29" s="11" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="N29" s="4"/>
     </row>
@@ -2247,19 +2247,19 @@
         <v>15</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I30" s="6" t="s">
         <v>19</v>
@@ -2268,13 +2268,13 @@
         <v>20</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L30" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="N30" s="9"/>
     </row>
@@ -2289,19 +2289,19 @@
         <v>15</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I31" s="6" t="s">
         <v>19</v>
@@ -2310,13 +2310,13 @@
         <v>20</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L31" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="N31" s="4"/>
     </row>
@@ -2331,19 +2331,19 @@
         <v>15</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G32" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="H32" s="13" t="s">
         <v>129</v>
-      </c>
-      <c r="H32" s="13" t="s">
-        <v>133</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>19</v>
@@ -2352,13 +2352,13 @@
         <v>20</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L32" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="N32" s="4"/>
     </row>
@@ -2373,19 +2373,19 @@
         <v>15</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I33" s="6" t="s">
         <v>19</v>
@@ -2394,13 +2394,13 @@
         <v>20</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L33" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="N33" s="4"/>
     </row>

</xml_diff>

<commit_message>
Added zip_code tests (boundary values)
</commit_message>
<xml_diff>
--- a/docs/GE3_TestCasesTemplate_2023_v1.0.xlsx
+++ b/docs/GE3_TestCasesTemplate_2023_v1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edu/PycharmProjects/G89.2023.T20.EG3/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\OneDrive\Escritorio\Desarrollo de Software\G89.2023.T20.EG3\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2523F5-9EC0-1D4B-B369-5BCAA22CE6E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C1E785-5C35-4968-9CDA-1174585EE0F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="500" windowWidth="27720" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="503" windowWidth="27720" windowHeight="17498" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GE3 2023 F1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="159">
   <si>
     <t>#</t>
   </si>
@@ -319,6 +319,9 @@
     <t>"C/LISBOA MARINERA,4, MADRID, SPAIN"</t>
   </si>
   <si>
+    <t>CALLE DE NUESTRO SEÑOR SATORU GOJO EL BENEVOLENTE QUE CON SUS ARTES MARCIALES NATURAL, MADRID, ESPAÑA</t>
+  </si>
+  <si>
     <t>LV</t>
   </si>
   <si>
@@ -475,7 +478,37 @@
     <t>Exception: Zip code not valid, must be numeric in the range {01000-52999}</t>
   </si>
   <si>
-    <t>"Calle de la Gran Via de Madrid, Madrid, Madrid, Madrid, Madrid, Madrid, Madrid, Madrid, Madrid, Madri"</t>
+    <t>ZIP_CODE Exactly 01000</t>
+  </si>
+  <si>
+    <t>ZIP_CODE Exactly 52999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALID </t>
+  </si>
+  <si>
+    <t>"01000"</t>
+  </si>
+  <si>
+    <t>"52999"</t>
+  </si>
+  <si>
+    <t>ZIP_CODE One above 01000</t>
+  </si>
+  <si>
+    <t>ZIP_CODE One below 52999</t>
+  </si>
+  <si>
+    <t>Exception: Zip code not valid, must be less than 53001</t>
+  </si>
+  <si>
+    <t>Exception: Zip code not valid, must be less than 53002</t>
+  </si>
+  <si>
+    <t>"01001"</t>
+  </si>
+  <si>
+    <t>"52998"</t>
   </si>
 </sst>
 </file>
@@ -550,7 +583,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -587,6 +620,30 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FFD9E2F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFD9E2F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -600,7 +657,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -623,6 +680,10 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -730,7 +791,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:N51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:N47">
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="I/O"/>
@@ -982,28 +1043,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD1008"/>
+  <dimension ref="A1:AD1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M57" sqref="M57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.1640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.71875" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="47.7109375" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="56.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="30" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="47.71875" customWidth="1"/>
+    <col min="11" max="11" width="17.71875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="56.71875" bestFit="1" customWidth="1"/>
+    <col min="14" max="30" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="15.75" customHeight="1">
@@ -1079,7 +1140,7 @@
       <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="16" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="5" t="s">
@@ -1089,7 +1150,7 @@
         <v>18</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>19</v>
@@ -1121,7 +1182,7 @@
       <c r="D3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F3" s="5" t="s">
@@ -1131,7 +1192,7 @@
         <v>44</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>24</v>
@@ -1163,7 +1224,7 @@
       <c r="D4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -1173,7 +1234,7 @@
         <v>26</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>19</v>
@@ -1200,12 +1261,12 @@
         <v>14</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -1215,7 +1276,7 @@
         <v>78</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>19</v>
@@ -1242,12 +1303,12 @@
         <v>14</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -1257,7 +1318,7 @@
         <v>79</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>19</v>
@@ -1289,7 +1350,7 @@
       <c r="D7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="16" t="s">
         <v>16</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -1299,7 +1360,7 @@
         <v>89</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>19</v>
@@ -1331,17 +1392,17 @@
       <c r="D8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="16" t="s">
         <v>16</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>89</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>24</v>
@@ -1373,7 +1434,7 @@
       <c r="D9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -1383,7 +1444,7 @@
         <v>91</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>90</v>
@@ -1398,7 +1459,7 @@
         <v>21</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="N9" s="4"/>
     </row>
@@ -1415,7 +1476,7 @@
       <c r="D10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -1425,7 +1486,7 @@
         <v>45</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I10" s="6">
         <v>123</v>
@@ -1440,7 +1501,7 @@
         <v>21</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="N10" s="4"/>
     </row>
@@ -1457,17 +1518,17 @@
       <c r="D11" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="16" t="s">
         <v>16</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>88</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>19</v>
@@ -1494,22 +1555,22 @@
         <v>14</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="16" t="s">
         <v>16</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>92</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>19</v>
@@ -1536,12 +1597,12 @@
         <v>14</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="16" t="s">
         <v>16</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -1551,7 +1612,7 @@
         <v>93</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>19</v>
@@ -1578,12 +1639,12 @@
         <v>14</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F14" s="5" t="s">
@@ -1593,7 +1654,7 @@
         <v>49</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>19</v>
@@ -1608,7 +1669,7 @@
         <v>21</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="N14" s="4"/>
     </row>
@@ -1625,7 +1686,7 @@
       <c r="D15" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F15" s="5" t="s">
@@ -1635,7 +1696,7 @@
         <v>52</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>19</v>
@@ -1650,7 +1711,7 @@
         <v>21</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="N15" s="4"/>
     </row>
@@ -1662,12 +1723,12 @@
         <v>14</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F16" s="5" t="s">
@@ -1677,7 +1738,7 @@
         <v>54</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>19</v>
@@ -1692,7 +1753,7 @@
         <v>21</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="N16" s="4"/>
     </row>
@@ -1704,12 +1765,12 @@
         <v>14</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F17" s="5" t="s">
@@ -1719,13 +1780,13 @@
         <v>57</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>19</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="K17" s="6" t="s">
         <v>77</v>
@@ -1734,7 +1795,7 @@
         <v>21</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="N17" s="4"/>
     </row>
@@ -1751,17 +1812,17 @@
       <c r="D18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="19" t="s">
         <v>22</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>62</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>19</v>
@@ -1793,7 +1854,7 @@
       <c r="D19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="19" t="s">
         <v>22</v>
       </c>
       <c r="F19" s="4" t="s">
@@ -1803,7 +1864,7 @@
         <v>61</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>19</v>
@@ -1818,7 +1879,7 @@
         <v>21</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="N19" s="4"/>
     </row>
@@ -1835,7 +1896,7 @@
       <c r="D20" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="17" t="s">
         <v>65</v>
       </c>
       <c r="F20" s="4" t="s">
@@ -1845,7 +1906,7 @@
         <v>67</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>19</v>
@@ -1854,7 +1915,7 @@
         <v>20</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="L20" s="11" t="s">
         <v>21</v>
@@ -1877,17 +1938,17 @@
       <c r="D21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="19" t="s">
         <v>22</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>69</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>19</v>
@@ -1896,13 +1957,13 @@
         <v>20</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L21" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M21" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N21" s="4"/>
     </row>
@@ -1919,17 +1980,17 @@
       <c r="D22" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="19" t="s">
         <v>22</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>70</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>19</v>
@@ -1938,13 +1999,13 @@
         <v>20</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L22" s="11" t="s">
         <v>21</v>
       </c>
       <c r="M22" s="10" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="N22" s="4"/>
     </row>
@@ -1961,17 +2022,17 @@
       <c r="D23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="19" t="s">
         <v>22</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>19</v>
@@ -2003,17 +2064,17 @@
       <c r="D24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="17" t="s">
         <v>16</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>18</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>19</v>
@@ -2040,22 +2101,22 @@
         <v>14</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="19" t="s">
         <v>71</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>72</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>19</v>
@@ -2067,10 +2128,10 @@
         <v>77</v>
       </c>
       <c r="L25" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N25" s="4"/>
     </row>
@@ -2082,22 +2143,22 @@
         <v>14</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="19" t="s">
         <v>71</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>19</v>
@@ -2109,10 +2170,10 @@
         <v>77</v>
       </c>
       <c r="L26" s="11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N26" s="4"/>
     </row>
@@ -2124,22 +2185,22 @@
         <v>14</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="19" t="s">
         <v>71</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>19</v>
@@ -2151,10 +2212,10 @@
         <v>77</v>
       </c>
       <c r="L27" s="11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="N27" s="4"/>
     </row>
@@ -2166,22 +2227,22 @@
         <v>14</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="19" t="s">
         <v>71</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>74</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>19</v>
@@ -2193,10 +2254,10 @@
         <v>77</v>
       </c>
       <c r="L28" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="N28" s="4"/>
     </row>
@@ -2213,17 +2274,17 @@
       <c r="D29" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="19" t="s">
         <v>71</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>75</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I29" s="6" t="s">
         <v>19</v>
@@ -2238,7 +2299,7 @@
         <v>76</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="N29" s="4"/>
     </row>
@@ -2247,294 +2308,413 @@
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="6"/>
-      <c r="N30" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="L30" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M30" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="N30" s="9"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1">
       <c r="A31" s="4">
         <v>30</v>
       </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="6"/>
+      <c r="B31" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="L31" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>119</v>
+      </c>
       <c r="N31" s="4"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1">
       <c r="A32" s="4">
         <v>31</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="6"/>
+      <c r="B32" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="L32" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>119</v>
+      </c>
       <c r="N32" s="4"/>
     </row>
     <row r="33" spans="1:14" ht="15.75" customHeight="1">
       <c r="A33" s="4">
         <v>32</v>
       </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="6"/>
+      <c r="B33" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="L33" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M33" s="6" t="s">
+        <v>119</v>
+      </c>
       <c r="N33" s="4"/>
     </row>
     <row r="34" spans="1:14" ht="15.75" customHeight="1">
-      <c r="B34" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E34" s="4" t="s">
+      <c r="A34" s="4">
+        <v>33</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="4"/>
+    </row>
+    <row r="35" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A35" s="4">
+        <v>34</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+    </row>
+    <row r="36" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A36" s="4">
+        <v>35</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+    </row>
+    <row r="37" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A37" s="4">
+        <v>36</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+    </row>
+    <row r="38" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A38" s="4">
+        <v>37</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="L38" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="M38" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="N38" s="4"/>
+    </row>
+    <row r="39" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A39" s="4">
+        <v>38</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="L39" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="N39" s="4"/>
+    </row>
+    <row r="40" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A40" s="4">
+        <v>39</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="F34" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="H34" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="I34" s="6" t="s">
+      <c r="F40" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="I40" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J34" s="6" t="s">
+      <c r="J40" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K34" s="6" t="s">
+      <c r="K40" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="L34" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="M34" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="N34" s="9"/>
-    </row>
-    <row r="35" spans="1:14" ht="15.75" customHeight="1">
-      <c r="B35" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E35" s="4" t="s">
+      <c r="L40" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="M40" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="N40" s="4"/>
+    </row>
+    <row r="41" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A41" s="4">
+        <v>40</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="F35" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H35" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="I35" s="6" t="s">
+      <c r="F41" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="I41" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J35" s="6" t="s">
+      <c r="J41" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K35" s="6" t="s">
+      <c r="K41" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="L35" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="M35" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="N35" s="4"/>
-    </row>
-    <row r="36" spans="1:14" ht="15.75" customHeight="1">
-      <c r="B36" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="H36" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="I36" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J36" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K36" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="L36" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="M36" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="N36" s="4"/>
-    </row>
-    <row r="37" spans="1:14" ht="15.75" customHeight="1">
-      <c r="B37" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="H37" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J37" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K37" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="L37" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="M37" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="N37" s="4"/>
-    </row>
-    <row r="38" spans="1:14" ht="15.75" customHeight="1">
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="12"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="4"/>
-    </row>
-    <row r="39" spans="1:14" ht="15.75" customHeight="1">
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-    </row>
-    <row r="40" spans="1:14" ht="15.75" customHeight="1">
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
-    </row>
-    <row r="41" spans="1:14" ht="15.75" customHeight="1">
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
+      <c r="L41" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="M41" s="6" t="s">
+        <v>156</v>
+      </c>
       <c r="N41" s="4"/>
     </row>
     <row r="42" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A42" s="4">
+        <v>41</v>
+      </c>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
@@ -2550,7 +2730,9 @@
       <c r="N42" s="4"/>
     </row>
     <row r="43" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A43" s="4"/>
+      <c r="A43" s="4">
+        <v>42</v>
+      </c>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
@@ -2566,7 +2748,9 @@
       <c r="N43" s="4"/>
     </row>
     <row r="44" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A44" s="4"/>
+      <c r="A44" s="4">
+        <v>43</v>
+      </c>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
@@ -2629,83 +2813,23 @@
       <c r="M47" s="4"/>
       <c r="N47" s="4"/>
     </row>
-    <row r="48" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4"/>
-    </row>
-    <row r="49" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-    </row>
-    <row r="50" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
-      <c r="L50" s="4"/>
-      <c r="M50" s="4"/>
-      <c r="N50" s="4"/>
-    </row>
-    <row r="51" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A51" s="4"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
-      <c r="H51" s="4"/>
-      <c r="I51" s="4"/>
-      <c r="J51" s="4"/>
-      <c r="K51" s="4"/>
-      <c r="L51" s="4"/>
-      <c r="M51" s="4"/>
-      <c r="N51" s="4"/>
-    </row>
-    <row r="52" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="53" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="54" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="55" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="56" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="57" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="58" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="59" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="60" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="61" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="62" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="63" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="64" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="49" ht="15.75" customHeight="1"/>
+    <row r="50" ht="15.75" customHeight="1"/>
+    <row r="51" ht="15.75" customHeight="1"/>
+    <row r="52" ht="15.75" customHeight="1"/>
+    <row r="53" ht="15.75" customHeight="1"/>
+    <row r="54" ht="15.75" customHeight="1"/>
+    <row r="55" ht="15.75" customHeight="1"/>
+    <row r="56" ht="15.75" customHeight="1"/>
+    <row r="57" ht="15.75" customHeight="1"/>
+    <row r="58" ht="15.75" customHeight="1"/>
+    <row r="59" ht="15.75" customHeight="1"/>
+    <row r="60" ht="15.75" customHeight="1"/>
+    <row r="61" ht="15.75" customHeight="1"/>
+    <row r="62" ht="15.75" customHeight="1"/>
+    <row r="63" ht="15.75" customHeight="1"/>
+    <row r="64" ht="15.75" customHeight="1"/>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1"/>
@@ -3646,10 +3770,6 @@
     <row r="1002" ht="15.75" customHeight="1"/>
     <row r="1003" ht="15.75" customHeight="1"/>
     <row r="1004" ht="15.75" customHeight="1"/>
-    <row r="1005" ht="15.75" customHeight="1"/>
-    <row r="1006" ht="15.75" customHeight="1"/>
-    <row r="1007" ht="15.75" customHeight="1"/>
-    <row r="1008" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -3667,17 +3787,17 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.1640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
-    <col min="4" max="4" width="44.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="62.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" customWidth="1"/>
-    <col min="8" max="8" width="36.7109375" customWidth="1"/>
-    <col min="9" max="10" width="33.7109375" customWidth="1"/>
-    <col min="11" max="28" width="10.5703125" customWidth="1"/>
+    <col min="1" max="2" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" customWidth="1"/>
+    <col min="4" max="4" width="44.1640625" customWidth="1"/>
+    <col min="5" max="5" width="22.27734375" customWidth="1"/>
+    <col min="6" max="6" width="62.27734375" customWidth="1"/>
+    <col min="7" max="7" width="9.27734375" customWidth="1"/>
+    <col min="8" max="8" width="36.71875" customWidth="1"/>
+    <col min="9" max="10" width="33.71875" customWidth="1"/>
+    <col min="11" max="28" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="33" customHeight="1">
@@ -5232,15 +5352,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.1640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="62.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" customWidth="1"/>
-    <col min="6" max="7" width="33.7109375" customWidth="1"/>
-    <col min="8" max="25" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="22.27734375" customWidth="1"/>
+    <col min="4" max="4" width="62.27734375" customWidth="1"/>
+    <col min="5" max="5" width="9.27734375" customWidth="1"/>
+    <col min="6" max="7" width="33.71875" customWidth="1"/>
+    <col min="8" max="25" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1">

</xml_diff>